<commit_message>
Work for deployment in WSL
</commit_message>
<xml_diff>
--- a/testing/generate_face_log.xlsx
+++ b/testing/generate_face_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,43 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>222</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.1018543243408203</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-04-22 04:15:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>222</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.079498291015625</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-04-22 04:15:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>222</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>0.5246345996856689</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-03-30 00:48:32</t>
+      <c r="B4" t="n">
+        <v>0.05739951133728027</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-04-22 04:15:41</t>
         </is>
       </c>
     </row>

</xml_diff>